<commit_message>
Fixed Charge Pumps and Added Text
</commit_message>
<xml_diff>
--- a/BOMs/Plane_Project_Digikey_BOM_V2.xlsx
+++ b/BOMs/Plane_Project_Digikey_BOM_V2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adite\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caltech\SeniorYear\PlaneProject\GitFiles\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Index</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Extended Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -182,6 +185,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -539,13 +543,13 @@
         <v>11</v>
       </c>
       <c r="E3" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>0.1</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G3" s="4">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -677,13 +681,13 @@
         <v>26</v>
       </c>
       <c r="E9" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>0.08</v>
       </c>
       <c r="G9" s="4">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -753,6 +757,15 @@
       </c>
       <c r="G12" s="4">
         <v>0.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4">
+        <f>SUM(G2:G12)</f>
+        <v>12.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>